<commit_message>
cleanup for macroalgae analyses
</commit_message>
<xml_diff>
--- a/cross_dataset_comparisons/output/seabird-microbes/Table_SX_clean_microbiome.xlsx
+++ b/cross_dataset_comparisons/output/seabird-microbes/Table_SX_clean_microbiome.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannah/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannah/Documents/OSUDocs/Projects/French_Polynesia/Tetiaroa/Island_Survey/TARP_motu_comparison/cross_dataset_comparisons/output/seabird-microbes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB69201A-7FC3-A744-B1E9-C3E9C4A3FF39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B2F3A3-1761-D84F-80D3-767069CF1311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="520" windowWidth="28040" windowHeight="16300" activeTab="1" xr2:uid="{4FB2862D-2AED-284B-B8B7-6F6128E0CB7B}"/>
+    <workbookView xWindow="2180" yWindow="700" windowWidth="28040" windowHeight="16300" activeTab="1" xr2:uid="{4FB2862D-2AED-284B-B8B7-6F6128E0CB7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Microbiome Univariate Results" sheetId="6" r:id="rId1"/>
@@ -530,7 +530,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -581,12 +581,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -598,11 +592,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -939,7 +937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9F28309-32C8-5E47-A359-FFA5276B7D30}">
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
@@ -960,20 +958,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -2882,7 +2880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD79A22-9206-4C47-A3DF-875AF2E44DC7}">
   <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
       <selection activeCell="K83" sqref="K83"/>
     </sheetView>
   </sheetViews>
@@ -2895,14 +2893,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -3045,7 +3043,7 @@
       <c r="G8" s="7">
         <v>2.0203000000000002</v>
       </c>
-      <c r="H8" s="48">
+      <c r="H8">
         <v>1</v>
       </c>
       <c r="I8" s="8">
@@ -3060,7 +3058,7 @@
       <c r="G9" s="7">
         <v>2.02033</v>
       </c>
-      <c r="H9" s="48">
+      <c r="H9">
         <v>3</v>
       </c>
       <c r="I9" s="8">
@@ -3075,7 +3073,7 @@
       <c r="G10" s="7">
         <v>1.3813</v>
       </c>
-      <c r="H10" s="48">
+      <c r="H10">
         <v>1</v>
       </c>
       <c r="I10" s="8">
@@ -3120,7 +3118,7 @@
       <c r="G12" s="7">
         <v>0.81969999999999998</v>
       </c>
-      <c r="H12" s="48">
+      <c r="H12">
         <v>1</v>
       </c>
       <c r="I12" s="8">
@@ -3135,7 +3133,7 @@
       <c r="G13" s="7">
         <v>4.0997000000000003</v>
       </c>
-      <c r="H13" s="48">
+      <c r="H13">
         <v>3</v>
       </c>
       <c r="I13" s="8">
@@ -3150,7 +3148,7 @@
       <c r="G14" s="7">
         <v>2.46E-2</v>
       </c>
-      <c r="H14" s="48">
+      <c r="H14">
         <v>1</v>
       </c>
       <c r="I14" s="8">
@@ -3174,13 +3172,13 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="35" t="s">
         <v>67</v>
       </c>
       <c r="D16" s="5" t="s">
@@ -3189,16 +3187,16 @@
       <c r="E16" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F16" s="38" t="s">
+      <c r="F16" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="36">
+      <c r="G16" s="34">
         <v>3.6021999999999998</v>
       </c>
-      <c r="H16" s="39">
-        <v>1</v>
-      </c>
-      <c r="I16" s="40">
+      <c r="H16" s="37">
+        <v>1</v>
+      </c>
+      <c r="I16" s="38">
         <v>5.7700000000000001E-2</v>
       </c>
       <c r="J16" t="s">
@@ -3206,70 +3204,70 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="41"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="42" t="s">
+      <c r="A17" s="39"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="G17" s="41">
+      <c r="G17" s="39">
         <v>2.2404999999999999</v>
       </c>
-      <c r="H17" s="39">
-        <v>3</v>
-      </c>
-      <c r="I17" s="40">
+      <c r="H17" s="37">
+        <v>3</v>
+      </c>
+      <c r="I17" s="38">
         <v>0.52400000000000002</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="41"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="42" t="s">
+      <c r="A18" s="39"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="41">
+      <c r="G18" s="39">
         <v>0.67920000000000003</v>
       </c>
-      <c r="H18" s="39">
-        <v>1</v>
-      </c>
-      <c r="I18" s="40">
+      <c r="H18" s="37">
+        <v>1</v>
+      </c>
+      <c r="I18" s="38">
         <v>0.40989999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="41"/>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="42" t="s">
+      <c r="A19" s="39"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="G19" s="45">
+      <c r="G19" s="43">
         <v>2.3978000000000002</v>
       </c>
-      <c r="H19" s="43">
-        <v>3</v>
-      </c>
-      <c r="I19" s="44">
+      <c r="H19" s="41">
+        <v>3</v>
+      </c>
+      <c r="I19" s="42">
         <v>0.49399999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="37" t="s">
+      <c r="B20" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="37" t="s">
+      <c r="C20" s="35" t="s">
         <v>66</v>
       </c>
       <c r="D20" s="5" t="s">
@@ -3278,84 +3276,84 @@
       <c r="E20" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F20" s="38" t="s">
+      <c r="F20" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="G20" s="36">
+      <c r="G20" s="34">
         <v>0.29899999999999999</v>
       </c>
-      <c r="H20" s="39">
-        <v>1</v>
-      </c>
-      <c r="I20" s="40">
+      <c r="H20" s="37">
+        <v>1</v>
+      </c>
+      <c r="I20" s="38">
         <v>0.58450000000000002</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="41"/>
-      <c r="B21" s="39"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="42" t="s">
+      <c r="A21" s="39"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="G21" s="41">
+      <c r="G21" s="39">
         <v>1.3519000000000001</v>
       </c>
-      <c r="H21" s="39">
-        <v>3</v>
-      </c>
-      <c r="I21" s="40">
+      <c r="H21" s="37">
+        <v>3</v>
+      </c>
+      <c r="I21" s="38">
         <v>0.71679999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="41"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="42" t="s">
+      <c r="A22" s="39"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="G22" s="41">
+      <c r="G22" s="39">
         <v>1.1680999999999999</v>
       </c>
-      <c r="H22" s="39">
-        <v>1</v>
-      </c>
-      <c r="I22" s="40">
+      <c r="H22" s="37">
+        <v>1</v>
+      </c>
+      <c r="I22" s="38">
         <v>0.27979999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="41"/>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="42" t="s">
+      <c r="A23" s="39"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="G23" s="45">
+      <c r="G23" s="43">
         <v>6.6100000000000006E-2</v>
       </c>
-      <c r="H23" s="43">
-        <v>3</v>
-      </c>
-      <c r="I23" s="44">
+      <c r="H23" s="41">
+        <v>3</v>
+      </c>
+      <c r="I23" s="42">
         <v>0.99560000000000004</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="36" t="s">
+      <c r="A24" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="37" t="s">
+      <c r="C24" s="35" t="s">
         <v>64</v>
       </c>
       <c r="D24" s="5" t="s">
@@ -3364,84 +3362,84 @@
       <c r="E24" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F24" s="38" t="s">
+      <c r="F24" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="G24" s="36">
+      <c r="G24" s="34">
         <v>1.2231000000000001</v>
       </c>
-      <c r="H24" s="39">
-        <v>1</v>
-      </c>
-      <c r="I24" s="40">
+      <c r="H24" s="37">
+        <v>1</v>
+      </c>
+      <c r="I24" s="38">
         <v>0.26869999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="41"/>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="42" t="s">
+      <c r="A25" s="39"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="G25" s="41">
+      <c r="G25" s="39">
         <v>0.62890000000000001</v>
       </c>
-      <c r="H25" s="39">
-        <v>3</v>
-      </c>
-      <c r="I25" s="40">
+      <c r="H25" s="37">
+        <v>3</v>
+      </c>
+      <c r="I25" s="38">
         <v>0.88980000000000004</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="41"/>
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="42" t="s">
+      <c r="A26" s="39"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="G26" s="41">
+      <c r="G26" s="39">
         <v>1.1778999999999999</v>
       </c>
-      <c r="H26" s="39">
-        <v>1</v>
-      </c>
-      <c r="I26" s="40">
+      <c r="H26" s="37">
+        <v>1</v>
+      </c>
+      <c r="I26" s="38">
         <v>0.27779999999999999</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="41"/>
-      <c r="B27" s="39"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="42" t="s">
+      <c r="A27" s="39"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="G27" s="45">
+      <c r="G27" s="43">
         <v>0.25990000000000002</v>
       </c>
-      <c r="H27" s="43">
-        <v>3</v>
-      </c>
-      <c r="I27" s="44">
+      <c r="H27" s="41">
+        <v>3</v>
+      </c>
+      <c r="I27" s="42">
         <v>0.96740000000000004</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="37" t="s">
+      <c r="B28" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="37" t="s">
+      <c r="C28" s="35" t="s">
         <v>65</v>
       </c>
       <c r="D28" s="5" t="s">
@@ -3450,84 +3448,84 @@
       <c r="E28" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F28" s="38" t="s">
+      <c r="F28" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="G28" s="41">
+      <c r="G28" s="39">
         <v>0.18820000000000001</v>
       </c>
-      <c r="H28" s="39">
-        <v>1</v>
-      </c>
-      <c r="I28" s="40">
+      <c r="H28" s="37">
+        <v>1</v>
+      </c>
+      <c r="I28" s="38">
         <v>0.66439999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="41"/>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="42" t="s">
+      <c r="A29" s="39"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="G29" s="41">
+      <c r="G29" s="39">
         <v>1.3206</v>
       </c>
-      <c r="H29" s="39">
-        <v>3</v>
-      </c>
-      <c r="I29" s="40">
+      <c r="H29" s="37">
+        <v>3</v>
+      </c>
+      <c r="I29" s="38">
         <v>0.72419999999999995</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="41"/>
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="42" t="s">
+      <c r="A30" s="39"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="G30" s="41">
+      <c r="G30" s="39">
         <v>0.2059</v>
       </c>
-      <c r="H30" s="39">
-        <v>1</v>
-      </c>
-      <c r="I30" s="40">
+      <c r="H30" s="37">
+        <v>1</v>
+      </c>
+      <c r="I30" s="38">
         <v>0.65</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="41"/>
-      <c r="B31" s="39"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="42" t="s">
+      <c r="A31" s="39"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="G31" s="45">
+      <c r="G31" s="43">
         <v>1.5206</v>
       </c>
-      <c r="H31" s="43">
-        <v>3</v>
-      </c>
-      <c r="I31" s="44">
+      <c r="H31" s="41">
+        <v>3</v>
+      </c>
+      <c r="I31" s="42">
         <v>0.67749999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="37" t="s">
+      <c r="C32" s="35" t="s">
         <v>63</v>
       </c>
       <c r="D32" s="5" t="s">
@@ -3536,84 +3534,84 @@
       <c r="E32" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F32" s="38" t="s">
+      <c r="F32" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="G32" s="36">
+      <c r="G32" s="34">
         <v>0.34150000000000003</v>
       </c>
-      <c r="H32" s="39">
-        <v>1</v>
-      </c>
-      <c r="I32" s="40">
+      <c r="H32" s="37">
+        <v>1</v>
+      </c>
+      <c r="I32" s="38">
         <v>0.55900000000000005</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="41"/>
-      <c r="B33" s="39"/>
-      <c r="C33" s="39"/>
-      <c r="D33" s="39"/>
-      <c r="E33" s="39"/>
-      <c r="F33" s="42" t="s">
+      <c r="A33" s="39"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="G33" s="41">
+      <c r="G33" s="39">
         <v>1.0506</v>
       </c>
-      <c r="H33" s="39">
-        <v>3</v>
-      </c>
-      <c r="I33" s="40">
+      <c r="H33" s="37">
+        <v>3</v>
+      </c>
+      <c r="I33" s="38">
         <v>0.78900000000000003</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="41"/>
-      <c r="B34" s="39"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="42" t="s">
+      <c r="A34" s="39"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="G34" s="41">
+      <c r="G34" s="39">
         <v>6.6E-3</v>
       </c>
-      <c r="H34" s="39">
-        <v>1</v>
-      </c>
-      <c r="I34" s="40">
+      <c r="H34" s="37">
+        <v>1</v>
+      </c>
+      <c r="I34" s="38">
         <v>0.93500000000000005</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="41"/>
-      <c r="B35" s="39"/>
-      <c r="C35" s="39"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="42" t="s">
+      <c r="A35" s="39"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="G35" s="45">
+      <c r="G35" s="43">
         <v>0.33689999999999998</v>
       </c>
-      <c r="H35" s="43">
-        <v>3</v>
-      </c>
-      <c r="I35" s="44">
+      <c r="H35" s="41">
+        <v>3</v>
+      </c>
+      <c r="I35" s="42">
         <v>0.95289999999999997</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="36" t="s">
+      <c r="A36" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="B36" s="37" t="s">
+      <c r="B36" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C36" s="37" t="s">
+      <c r="C36" s="35" t="s">
         <v>54</v>
       </c>
       <c r="D36" s="5" t="s">
@@ -3622,35 +3620,35 @@
       <c r="E36" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F36" s="38" t="s">
+      <c r="F36" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="G36" s="41">
+      <c r="G36" s="39">
         <v>2.3852000000000002</v>
       </c>
-      <c r="H36" s="39">
-        <v>1</v>
-      </c>
-      <c r="I36" s="40">
+      <c r="H36" s="37">
+        <v>1</v>
+      </c>
+      <c r="I36" s="38">
         <v>0.12249</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37" s="41"/>
-      <c r="B37" s="39"/>
-      <c r="C37" s="39"/>
-      <c r="D37" s="39"/>
-      <c r="E37" s="39"/>
-      <c r="F37" s="42" t="s">
+      <c r="A37" s="39"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="G37" s="41">
+      <c r="G37" s="39">
         <v>7.6753</v>
       </c>
-      <c r="H37" s="39">
-        <v>3</v>
-      </c>
-      <c r="I37" s="40">
+      <c r="H37" s="37">
+        <v>3</v>
+      </c>
+      <c r="I37" s="38">
         <v>5.3220000000000003E-2</v>
       </c>
       <c r="J37" t="s">
@@ -3658,69 +3656,69 @@
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38" s="41"/>
-      <c r="B38" s="39"/>
-      <c r="C38" s="39"/>
-      <c r="D38" s="39"/>
-      <c r="E38" s="39"/>
-      <c r="F38" s="42" t="s">
+      <c r="A38" s="39"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="G38" s="41">
+      <c r="G38" s="39">
         <v>8.1199999999999994E-2</v>
       </c>
-      <c r="H38" s="39">
-        <v>1</v>
-      </c>
-      <c r="I38" s="40">
+      <c r="H38" s="37">
+        <v>1</v>
+      </c>
+      <c r="I38" s="38">
         <v>0.77566000000000002</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="45"/>
-      <c r="B39" s="43"/>
-      <c r="C39" s="43"/>
-      <c r="D39" s="43"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="46" t="s">
+      <c r="A39" s="43"/>
+      <c r="B39" s="41"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="41"/>
+      <c r="E39" s="41"/>
+      <c r="F39" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="G39" s="45">
+      <c r="G39" s="43">
         <v>3.4470999999999998</v>
       </c>
-      <c r="H39" s="43">
-        <v>3</v>
-      </c>
-      <c r="I39" s="44">
+      <c r="H39" s="41">
+        <v>3</v>
+      </c>
+      <c r="I39" s="42">
         <v>0.32768000000000003</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" s="36" t="s">
+      <c r="A40" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="B40" s="37" t="s">
+      <c r="B40" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="37" t="s">
+      <c r="C40" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="D40" s="37" t="s">
+      <c r="D40" s="35" t="s">
         <v>13</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F40" s="38" t="s">
+      <c r="F40" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="G40" s="41">
+      <c r="G40" s="39">
         <v>7.0084</v>
       </c>
-      <c r="H40" s="39">
-        <v>1</v>
-      </c>
-      <c r="I40" s="49">
+      <c r="H40" s="37">
+        <v>1</v>
+      </c>
+      <c r="I40" s="45">
         <v>8.1130000000000004E-3</v>
       </c>
       <c r="J40" t="s">
@@ -3728,21 +3726,21 @@
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41" s="41"/>
-      <c r="B41" s="39"/>
-      <c r="C41" s="39"/>
-      <c r="D41" s="39"/>
-      <c r="E41" s="39"/>
-      <c r="F41" s="42" t="s">
+      <c r="A41" s="39"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="G41" s="41">
+      <c r="G41" s="39">
         <v>21.8504</v>
       </c>
-      <c r="H41" s="39">
-        <v>3</v>
-      </c>
-      <c r="I41" s="50">
+      <c r="H41" s="37">
+        <v>3</v>
+      </c>
+      <c r="I41" s="46">
         <v>6.9999999999999994E-5</v>
       </c>
       <c r="J41" t="s">
@@ -3750,40 +3748,40 @@
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A42" s="41"/>
-      <c r="B42" s="39"/>
-      <c r="C42" s="39"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="39"/>
-      <c r="F42" s="42" t="s">
+      <c r="A42" s="39"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="37"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="G42" s="41">
+      <c r="G42" s="39">
         <v>0.50870000000000004</v>
       </c>
-      <c r="H42" s="39">
-        <v>1</v>
-      </c>
-      <c r="I42" s="40">
+      <c r="H42" s="37">
+        <v>1</v>
+      </c>
+      <c r="I42" s="38">
         <v>0.44604700000000003</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A43" s="45"/>
-      <c r="B43" s="43"/>
-      <c r="C43" s="43"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="46" t="s">
+      <c r="A43" s="43"/>
+      <c r="B43" s="41"/>
+      <c r="C43" s="41"/>
+      <c r="D43" s="41"/>
+      <c r="E43" s="41"/>
+      <c r="F43" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="G43" s="45">
+      <c r="G43" s="43">
         <v>1.5025999999999999</v>
       </c>
-      <c r="H43" s="43">
-        <v>3</v>
-      </c>
-      <c r="I43" s="44">
+      <c r="H43" s="41">
+        <v>3</v>
+      </c>
+      <c r="I43" s="42">
         <v>0.68168099999999998</v>
       </c>
     </row>
@@ -3841,7 +3839,7 @@
       <c r="C48" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D48" s="47" t="s">
+      <c r="D48" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E48" s="2" t="s">
@@ -3933,7 +3931,7 @@
       <c r="C52" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D52" s="47" t="s">
+      <c r="D52" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E52" s="2" t="s">
@@ -3945,7 +3943,7 @@
       <c r="G52" s="7">
         <v>0.13339999999999999</v>
       </c>
-      <c r="H52" s="48">
+      <c r="H52">
         <v>1</v>
       </c>
       <c r="I52" s="8">
@@ -3963,7 +3961,7 @@
       <c r="G53" s="7">
         <v>1.4724999999999999</v>
       </c>
-      <c r="H53" s="48">
+      <c r="H53">
         <v>3</v>
       </c>
       <c r="I53" s="8">
@@ -3978,7 +3976,7 @@
       <c r="G54" s="7">
         <v>2.35E-2</v>
       </c>
-      <c r="H54" s="48">
+      <c r="H54">
         <v>1</v>
       </c>
       <c r="I54" s="8">
@@ -4012,7 +4010,7 @@
       <c r="C56" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D56" s="47" t="s">
+      <c r="D56" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E56" s="2" t="s">
@@ -4024,7 +4022,7 @@
       <c r="G56" s="7">
         <v>0.82110000000000005</v>
       </c>
-      <c r="H56" s="48">
+      <c r="H56">
         <v>1</v>
       </c>
       <c r="I56" s="8">
@@ -4039,7 +4037,7 @@
       <c r="G57" s="7">
         <v>0.56169999999999998</v>
       </c>
-      <c r="H57" s="48">
+      <c r="H57">
         <v>3</v>
       </c>
       <c r="I57" s="8">
@@ -4054,7 +4052,7 @@
       <c r="G58" s="7">
         <v>1E-4</v>
       </c>
-      <c r="H58" s="48">
+      <c r="H58">
         <v>1</v>
       </c>
       <c r="I58" s="8">
@@ -4068,7 +4066,7 @@
       <c r="F59" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G59" s="51">
+      <c r="G59" s="47">
         <v>4.7781000000000002</v>
       </c>
       <c r="H59" s="12">
@@ -4088,7 +4086,7 @@
       <c r="C60" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D60" s="47" t="s">
+      <c r="D60" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E60" s="2" t="s">
@@ -4100,7 +4098,7 @@
       <c r="G60" s="7">
         <v>3.0999999999999999E-3</v>
       </c>
-      <c r="H60" s="48">
+      <c r="H60">
         <v>1</v>
       </c>
       <c r="I60" s="8">
@@ -4115,7 +4113,7 @@
       <c r="G61" s="7">
         <v>1.8563000000000001</v>
       </c>
-      <c r="H61" s="48">
+      <c r="H61">
         <v>3</v>
       </c>
       <c r="I61" s="8">
@@ -4130,7 +4128,7 @@
       <c r="G62" s="7">
         <v>0.29480000000000001</v>
       </c>
-      <c r="H62" s="48">
+      <c r="H62">
         <v>1</v>
       </c>
       <c r="I62" s="8">
@@ -4157,85 +4155,85 @@
       <c r="A64" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B64" s="37" t="s">
+      <c r="B64" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C64" s="37" t="s">
+      <c r="C64" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="D64" s="47" t="s">
+      <c r="D64" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E64" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="F64" s="38" t="s">
+      <c r="F64" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="G64" s="36">
+      <c r="G64" s="34">
         <v>0.97819999999999996</v>
       </c>
-      <c r="H64" s="39">
-        <v>1</v>
-      </c>
-      <c r="I64" s="40">
+      <c r="H64" s="37">
+        <v>1</v>
+      </c>
+      <c r="I64" s="38">
         <v>0.3226</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A65" s="41"/>
-      <c r="B65" s="39"/>
-      <c r="C65" s="39"/>
-      <c r="D65" s="39"/>
-      <c r="E65" s="39"/>
-      <c r="F65" s="42" t="s">
+      <c r="A65" s="39"/>
+      <c r="B65" s="37"/>
+      <c r="C65" s="37"/>
+      <c r="D65" s="37"/>
+      <c r="E65" s="37"/>
+      <c r="F65" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="G65" s="41">
+      <c r="G65" s="39">
         <v>1.2331000000000001</v>
       </c>
-      <c r="H65" s="39">
-        <v>3</v>
-      </c>
-      <c r="I65" s="40">
+      <c r="H65" s="37">
+        <v>3</v>
+      </c>
+      <c r="I65" s="38">
         <v>0.74509999999999998</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A66" s="41"/>
-      <c r="B66" s="39"/>
-      <c r="C66" s="39"/>
-      <c r="D66" s="39"/>
-      <c r="E66" s="39"/>
-      <c r="F66" s="42" t="s">
+      <c r="A66" s="39"/>
+      <c r="B66" s="37"/>
+      <c r="C66" s="37"/>
+      <c r="D66" s="37"/>
+      <c r="E66" s="37"/>
+      <c r="F66" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="G66" s="41">
+      <c r="G66" s="39">
         <v>0.1545</v>
       </c>
-      <c r="H66" s="39">
-        <v>1</v>
-      </c>
-      <c r="I66" s="40">
+      <c r="H66" s="37">
+        <v>1</v>
+      </c>
+      <c r="I66" s="38">
         <v>0.69430000000000003</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A67" s="45"/>
-      <c r="B67" s="39"/>
-      <c r="C67" s="39"/>
-      <c r="D67" s="43"/>
-      <c r="E67" s="39"/>
-      <c r="F67" s="42" t="s">
+      <c r="A67" s="43"/>
+      <c r="B67" s="37"/>
+      <c r="C67" s="37"/>
+      <c r="D67" s="41"/>
+      <c r="E67" s="37"/>
+      <c r="F67" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="G67" s="45">
+      <c r="G67" s="43">
         <v>0.71950000000000003</v>
       </c>
-      <c r="H67" s="43">
-        <v>3</v>
-      </c>
-      <c r="I67" s="44">
+      <c r="H67" s="41">
+        <v>3</v>
+      </c>
+      <c r="I67" s="42">
         <v>0.86860000000000004</v>
       </c>
     </row>
@@ -4243,85 +4241,85 @@
       <c r="A68" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B68" s="37" t="s">
+      <c r="B68" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C68" s="37" t="s">
+      <c r="C68" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="D68" s="47" t="s">
+      <c r="D68" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E68" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="F68" s="38" t="s">
+      <c r="F68" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="G68" s="41">
+      <c r="G68" s="39">
         <v>0.3306</v>
       </c>
-      <c r="H68" s="39">
-        <v>1</v>
-      </c>
-      <c r="I68" s="40">
+      <c r="H68" s="37">
+        <v>1</v>
+      </c>
+      <c r="I68" s="38">
         <v>0.56530000000000002</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A69" s="41"/>
-      <c r="B69" s="39"/>
-      <c r="C69" s="39"/>
-      <c r="D69" s="39"/>
-      <c r="E69" s="39"/>
-      <c r="F69" s="42" t="s">
+      <c r="A69" s="39"/>
+      <c r="B69" s="37"/>
+      <c r="C69" s="37"/>
+      <c r="D69" s="37"/>
+      <c r="E69" s="37"/>
+      <c r="F69" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="G69" s="41">
+      <c r="G69" s="39">
         <v>1.4674</v>
       </c>
-      <c r="H69" s="39">
-        <v>3</v>
-      </c>
-      <c r="I69" s="40">
+      <c r="H69" s="37">
+        <v>3</v>
+      </c>
+      <c r="I69" s="38">
         <v>0.68981999999999999</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A70" s="41"/>
-      <c r="B70" s="39"/>
-      <c r="C70" s="39"/>
-      <c r="D70" s="39"/>
-      <c r="E70" s="39"/>
-      <c r="F70" s="42" t="s">
+      <c r="A70" s="39"/>
+      <c r="B70" s="37"/>
+      <c r="C70" s="37"/>
+      <c r="D70" s="37"/>
+      <c r="E70" s="37"/>
+      <c r="F70" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="G70" s="41">
+      <c r="G70" s="39">
         <v>0.16339999999999999</v>
       </c>
-      <c r="H70" s="39">
-        <v>1</v>
-      </c>
-      <c r="I70" s="40">
+      <c r="H70" s="37">
+        <v>1</v>
+      </c>
+      <c r="I70" s="38">
         <v>0.68606</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A71" s="45"/>
-      <c r="B71" s="39"/>
-      <c r="C71" s="39"/>
-      <c r="D71" s="43"/>
-      <c r="E71" s="43"/>
-      <c r="F71" s="42" t="s">
+      <c r="A71" s="43"/>
+      <c r="B71" s="37"/>
+      <c r="C71" s="37"/>
+      <c r="D71" s="41"/>
+      <c r="E71" s="41"/>
+      <c r="F71" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="G71" s="45">
+      <c r="G71" s="43">
         <v>6.2563000000000004</v>
       </c>
-      <c r="H71" s="43">
-        <v>3</v>
-      </c>
-      <c r="I71" s="44">
+      <c r="H71" s="41">
+        <v>3</v>
+      </c>
+      <c r="I71" s="42">
         <v>9.9790000000000004E-2</v>
       </c>
     </row>
@@ -4329,85 +4327,85 @@
       <c r="A72" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B72" s="37" t="s">
+      <c r="B72" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C72" s="37" t="s">
+      <c r="C72" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="D72" s="47" t="s">
+      <c r="D72" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F72" s="38" t="s">
+      <c r="F72" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="G72" s="36">
+      <c r="G72" s="34">
         <v>0.1701</v>
       </c>
-      <c r="H72" s="39">
-        <v>1</v>
-      </c>
-      <c r="I72" s="40">
+      <c r="H72" s="37">
+        <v>1</v>
+      </c>
+      <c r="I72" s="38">
         <v>0.68</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A73" s="41"/>
-      <c r="B73" s="39"/>
-      <c r="C73" s="39"/>
-      <c r="D73" s="39"/>
-      <c r="E73" s="39"/>
-      <c r="F73" s="42" t="s">
+      <c r="A73" s="39"/>
+      <c r="B73" s="37"/>
+      <c r="C73" s="37"/>
+      <c r="D73" s="37"/>
+      <c r="E73" s="37"/>
+      <c r="F73" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="G73" s="41">
+      <c r="G73" s="39">
         <v>6.0106999999999999</v>
       </c>
-      <c r="H73" s="39">
-        <v>3</v>
-      </c>
-      <c r="I73" s="40">
+      <c r="H73" s="37">
+        <v>3</v>
+      </c>
+      <c r="I73" s="38">
         <v>0.1111</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A74" s="41"/>
-      <c r="B74" s="39"/>
-      <c r="C74" s="39"/>
-      <c r="D74" s="39"/>
-      <c r="E74" s="39"/>
-      <c r="F74" s="42" t="s">
+      <c r="A74" s="39"/>
+      <c r="B74" s="37"/>
+      <c r="C74" s="37"/>
+      <c r="D74" s="37"/>
+      <c r="E74" s="37"/>
+      <c r="F74" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="G74" s="41">
+      <c r="G74" s="39">
         <v>0.48759999999999998</v>
       </c>
-      <c r="H74" s="39">
-        <v>1</v>
-      </c>
-      <c r="I74" s="40">
+      <c r="H74" s="37">
+        <v>1</v>
+      </c>
+      <c r="I74" s="38">
         <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A75" s="45"/>
-      <c r="B75" s="39"/>
-      <c r="C75" s="39"/>
-      <c r="D75" s="43"/>
-      <c r="E75" s="39"/>
-      <c r="F75" s="42" t="s">
+      <c r="A75" s="43"/>
+      <c r="B75" s="37"/>
+      <c r="C75" s="37"/>
+      <c r="D75" s="41"/>
+      <c r="E75" s="37"/>
+      <c r="F75" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="G75" s="45">
+      <c r="G75" s="43">
         <v>1.1876</v>
       </c>
-      <c r="H75" s="43">
-        <v>3</v>
-      </c>
-      <c r="I75" s="44">
+      <c r="H75" s="41">
+        <v>3</v>
+      </c>
+      <c r="I75" s="42">
         <v>0.75600000000000001</v>
       </c>
     </row>
@@ -4415,85 +4413,85 @@
       <c r="A76" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B76" s="37" t="s">
+      <c r="B76" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C76" s="37" t="s">
+      <c r="C76" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="D76" s="47" t="s">
+      <c r="D76" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E76" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="F76" s="38" t="s">
+      <c r="F76" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="G76" s="41">
+      <c r="G76" s="39">
         <v>1.5900000000000001E-2</v>
       </c>
-      <c r="H76" s="39">
-        <v>1</v>
-      </c>
-      <c r="I76" s="40">
+      <c r="H76" s="37">
+        <v>1</v>
+      </c>
+      <c r="I76" s="38">
         <v>0.89980000000000004</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A77" s="41"/>
-      <c r="B77" s="39"/>
-      <c r="C77" s="39"/>
-      <c r="D77" s="39"/>
-      <c r="E77" s="39"/>
-      <c r="F77" s="42" t="s">
+      <c r="A77" s="39"/>
+      <c r="B77" s="37"/>
+      <c r="C77" s="37"/>
+      <c r="D77" s="37"/>
+      <c r="E77" s="37"/>
+      <c r="F77" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="G77" s="41">
+      <c r="G77" s="39">
         <v>2.4333999999999998</v>
       </c>
-      <c r="H77" s="39">
-        <v>3</v>
-      </c>
-      <c r="I77" s="40">
+      <c r="H77" s="37">
+        <v>3</v>
+      </c>
+      <c r="I77" s="38">
         <v>0.48743999999999998</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A78" s="41"/>
-      <c r="B78" s="39"/>
-      <c r="C78" s="39"/>
-      <c r="D78" s="39"/>
-      <c r="E78" s="39"/>
-      <c r="F78" s="42" t="s">
+      <c r="A78" s="39"/>
+      <c r="B78" s="37"/>
+      <c r="C78" s="37"/>
+      <c r="D78" s="37"/>
+      <c r="E78" s="37"/>
+      <c r="F78" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="G78" s="41">
+      <c r="G78" s="39">
         <v>2.9472999999999998</v>
       </c>
-      <c r="H78" s="39">
-        <v>1</v>
-      </c>
-      <c r="I78" s="40">
+      <c r="H78" s="37">
+        <v>1</v>
+      </c>
+      <c r="I78" s="38">
         <v>8.6019999999999999E-2</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A79" s="45"/>
-      <c r="B79" s="39"/>
-      <c r="C79" s="39"/>
-      <c r="D79" s="43"/>
-      <c r="E79" s="39"/>
-      <c r="F79" s="42" t="s">
+      <c r="A79" s="43"/>
+      <c r="B79" s="37"/>
+      <c r="C79" s="37"/>
+      <c r="D79" s="41"/>
+      <c r="E79" s="37"/>
+      <c r="F79" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="G79" s="45">
+      <c r="G79" s="43">
         <v>2.6295000000000002</v>
       </c>
-      <c r="H79" s="43">
-        <v>3</v>
-      </c>
-      <c r="I79" s="44">
+      <c r="H79" s="41">
+        <v>3</v>
+      </c>
+      <c r="I79" s="42">
         <v>0.45234000000000002</v>
       </c>
     </row>
@@ -4501,85 +4499,85 @@
       <c r="A80" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B80" s="37" t="s">
+      <c r="B80" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C80" s="37" t="s">
+      <c r="C80" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="D80" s="47" t="s">
+      <c r="D80" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E80" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="F80" s="38" t="s">
+      <c r="F80" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="G80" s="41">
+      <c r="G80" s="39">
         <v>1E-3</v>
       </c>
-      <c r="H80" s="39">
-        <v>1</v>
-      </c>
-      <c r="I80" s="40">
+      <c r="H80" s="37">
+        <v>1</v>
+      </c>
+      <c r="I80" s="38">
         <v>0.97460000000000002</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A81" s="41"/>
-      <c r="B81" s="39"/>
-      <c r="C81" s="39"/>
-      <c r="D81" s="39"/>
-      <c r="E81" s="39"/>
-      <c r="F81" s="42" t="s">
+      <c r="A81" s="39"/>
+      <c r="B81" s="37"/>
+      <c r="C81" s="37"/>
+      <c r="D81" s="37"/>
+      <c r="E81" s="37"/>
+      <c r="F81" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="G81" s="41">
+      <c r="G81" s="39">
         <v>0.87419999999999998</v>
       </c>
-      <c r="H81" s="39">
-        <v>3</v>
-      </c>
-      <c r="I81" s="40">
+      <c r="H81" s="37">
+        <v>3</v>
+      </c>
+      <c r="I81" s="38">
         <v>0.83169999999999999</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A82" s="41"/>
-      <c r="B82" s="39"/>
-      <c r="C82" s="39"/>
-      <c r="D82" s="39"/>
-      <c r="E82" s="39"/>
-      <c r="F82" s="42" t="s">
+      <c r="A82" s="39"/>
+      <c r="B82" s="37"/>
+      <c r="C82" s="37"/>
+      <c r="D82" s="37"/>
+      <c r="E82" s="37"/>
+      <c r="F82" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="G82" s="41">
+      <c r="G82" s="39">
         <v>0.27439999999999998</v>
       </c>
-      <c r="H82" s="39">
-        <v>1</v>
-      </c>
-      <c r="I82" s="40">
+      <c r="H82" s="37">
+        <v>1</v>
+      </c>
+      <c r="I82" s="38">
         <v>0.60040000000000004</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A83" s="45"/>
-      <c r="B83" s="39"/>
-      <c r="C83" s="39"/>
-      <c r="D83" s="43"/>
-      <c r="E83" s="39"/>
-      <c r="F83" s="42" t="s">
+      <c r="A83" s="43"/>
+      <c r="B83" s="37"/>
+      <c r="C83" s="37"/>
+      <c r="D83" s="41"/>
+      <c r="E83" s="37"/>
+      <c r="F83" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="G83" s="45">
+      <c r="G83" s="43">
         <v>0.66049999999999998</v>
       </c>
-      <c r="H83" s="43">
-        <v>3</v>
-      </c>
-      <c r="I83" s="44">
+      <c r="H83" s="41">
+        <v>3</v>
+      </c>
+      <c r="I83" s="42">
         <v>0.88249999999999995</v>
       </c>
     </row>
@@ -4587,85 +4585,85 @@
       <c r="A84" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B84" s="37" t="s">
+      <c r="B84" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C84" s="37" t="s">
+      <c r="C84" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="D84" s="47" t="s">
+      <c r="D84" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E84" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="F84" s="38" t="s">
+      <c r="F84" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="G84" s="41">
+      <c r="G84" s="39">
         <v>1.8700000000000001E-2</v>
       </c>
-      <c r="H84" s="39">
-        <v>1</v>
-      </c>
-      <c r="I84" s="40">
+      <c r="H84" s="37">
+        <v>1</v>
+      </c>
+      <c r="I84" s="38">
         <v>0.89139999999999997</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A85" s="41"/>
-      <c r="B85" s="39"/>
-      <c r="C85" s="39"/>
-      <c r="D85" s="39"/>
-      <c r="E85" s="39"/>
-      <c r="F85" s="42" t="s">
+      <c r="A85" s="39"/>
+      <c r="B85" s="37"/>
+      <c r="C85" s="37"/>
+      <c r="D85" s="37"/>
+      <c r="E85" s="37"/>
+      <c r="F85" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="G85" s="41">
+      <c r="G85" s="39">
         <v>1.6854</v>
       </c>
-      <c r="H85" s="39">
-        <v>3</v>
-      </c>
-      <c r="I85" s="40">
+      <c r="H85" s="37">
+        <v>3</v>
+      </c>
+      <c r="I85" s="38">
         <v>0.64019999999999999</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A86" s="41"/>
-      <c r="B86" s="39"/>
-      <c r="C86" s="39"/>
-      <c r="D86" s="39"/>
-      <c r="E86" s="39"/>
-      <c r="F86" s="42" t="s">
+      <c r="A86" s="39"/>
+      <c r="B86" s="37"/>
+      <c r="C86" s="37"/>
+      <c r="D86" s="37"/>
+      <c r="E86" s="37"/>
+      <c r="F86" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="G86" s="41">
+      <c r="G86" s="39">
         <v>3.32E-2</v>
       </c>
-      <c r="H86" s="39">
-        <v>1</v>
-      </c>
-      <c r="I86" s="40">
+      <c r="H86" s="37">
+        <v>1</v>
+      </c>
+      <c r="I86" s="38">
         <v>0.85540000000000005</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A87" s="45"/>
-      <c r="B87" s="43"/>
-      <c r="C87" s="43"/>
-      <c r="D87" s="43"/>
-      <c r="E87" s="43"/>
-      <c r="F87" s="46" t="s">
+      <c r="A87" s="43"/>
+      <c r="B87" s="41"/>
+      <c r="C87" s="41"/>
+      <c r="D87" s="41"/>
+      <c r="E87" s="41"/>
+      <c r="F87" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="G87" s="45">
+      <c r="G87" s="43">
         <v>0.3448</v>
       </c>
-      <c r="H87" s="43">
-        <v>3</v>
-      </c>
-      <c r="I87" s="44">
+      <c r="H87" s="41">
+        <v>3</v>
+      </c>
+      <c r="I87" s="42">
         <v>0.95140000000000002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cleanup for micro and macroalgae analyses and supplementary tables'
</commit_message>
<xml_diff>
--- a/cross_dataset_comparisons/output/seabird-microbes/Table_SX_clean_microbiome.xlsx
+++ b/cross_dataset_comparisons/output/seabird-microbes/Table_SX_clean_microbiome.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannah/Documents/OSUDocs/Projects/French_Polynesia/Tetiaroa/Island_Survey/TARP_motu_comparison/cross_dataset_comparisons/output/seabird-microbes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8EDE802-8AA3-8544-A27B-7B3C1DC9CEBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F3D2F1-2814-BE45-AD9C-FF90BEDD668F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7640" yWindow="720" windowWidth="28040" windowHeight="16300" activeTab="2" xr2:uid="{4FB2862D-2AED-284B-B8B7-6F6128E0CB7B}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16300" activeTab="1" xr2:uid="{4FB2862D-2AED-284B-B8B7-6F6128E0CB7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Microbiome Univariate Results" sheetId="6" r:id="rId1"/>
-    <sheet name="Top Taxa v N15 Results" sheetId="7" r:id="rId2"/>
-    <sheet name="Top Taxa v Status Results" sheetId="8" r:id="rId3"/>
+    <sheet name="Distlm bray v N15" sheetId="9" r:id="rId2"/>
+    <sheet name="Top Taxa v N15 Results" sheetId="7" r:id="rId3"/>
+    <sheet name="Top Taxa v Status Results" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="132">
   <si>
     <t>distribution</t>
   </si>
@@ -443,6 +444,82 @@
   </si>
   <si>
     <t>glmmTMB(RelAbund_Uncultured_Alteromonadaceae ~ reststat*Distance_to_shore + Exposure + (1|site.name), family = beta_family(), data = beta_trans_coral_microbiome, na.action = na.omit)</t>
+  </si>
+  <si>
+    <t>Distance based linear model</t>
+  </si>
+  <si>
+    <t>distance method</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>bray curtis</t>
+  </si>
+  <si>
+    <t>N15</t>
+  </si>
+  <si>
+    <t>distance.along.transect</t>
+  </si>
+  <si>
+    <t>exposure</t>
+  </si>
+  <si>
+    <t>N15: distance.along.transect</t>
+  </si>
+  <si>
+    <t>Residual</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Supplementary Table X:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Distance based linear model for nearshore a)coral and b)seawater microbial communities (using bray curtis dissimilarity) against N15 and distance along transect, using the adonis2() function from vegan in R. Adonis2 cannot handle random variables, so site name was not included. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Asterisk (*) indicates significant result at alpha = 0.05. </t>
+    </r>
+  </si>
+  <si>
+    <t>coral microbiome community</t>
+  </si>
+  <si>
+    <t>water microbiome</t>
+  </si>
+  <si>
+    <t>adonis2(bc.coral ~ algae.N15 * distance.along.transect  + Exposure,  data = coral.microbes.seabirds, method = "bray", permutations = 999, na.action = na.omit)</t>
+  </si>
+  <si>
+    <t>water microbiome community</t>
+  </si>
+  <si>
+    <t>adonis2(bc.water ~ algae.N15 * distance.along.transect  + Exposure,  data = water.microbes.seabirds, method = "bray", permutations = 999, na.action = na.omit)</t>
   </si>
 </sst>
 </file>
@@ -622,7 +699,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -687,15 +764,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -709,6 +777,21 @@
     </xf>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1045,8 +1128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9F28309-32C8-5E47-A359-FFA5276B7D30}">
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1066,20 +1149,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -2985,6 +3068,363 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C84D858-9AD8-2F4D-8080-3A2ABC675EC4}">
+  <dimension ref="A1:L15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="22.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="58" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4" t="s">
+        <v>120</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0.20979999999999999</v>
+      </c>
+      <c r="I4">
+        <v>1.1730000000000001E-2</v>
+      </c>
+      <c r="J4">
+        <v>0.71419999999999995</v>
+      </c>
+      <c r="K4" s="9">
+        <v>0.59599999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="7"/>
+      <c r="F5" t="s">
+        <v>121</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>0.67390000000000005</v>
+      </c>
+      <c r="I5">
+        <v>3.7679999999999998E-2</v>
+      </c>
+      <c r="J5">
+        <v>7.6490000000000002E-2</v>
+      </c>
+      <c r="K5" s="9">
+        <v>0.69699999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="7"/>
+      <c r="F6" t="s">
+        <v>122</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0.35489999999999999</v>
+      </c>
+      <c r="I6">
+        <v>1.984E-2</v>
+      </c>
+      <c r="J6">
+        <v>1.2083999999999999</v>
+      </c>
+      <c r="K6" s="9">
+        <v>0.248</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="7"/>
+      <c r="F7" t="s">
+        <v>123</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>1.0799000000000001</v>
+      </c>
+      <c r="I7">
+        <v>6.0389999999999999E-2</v>
+      </c>
+      <c r="J7">
+        <v>1.2258</v>
+      </c>
+      <c r="K7" s="9">
+        <v>0.25600000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="7"/>
+      <c r="F8" t="s">
+        <v>124</v>
+      </c>
+      <c r="G8">
+        <v>53</v>
+      </c>
+      <c r="H8">
+        <v>15.5649</v>
+      </c>
+      <c r="I8">
+        <v>0.87036000000000002</v>
+      </c>
+      <c r="K8" s="8"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="11"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="G9" s="12">
+        <v>61</v>
+      </c>
+      <c r="H9" s="12">
+        <v>17.883400000000002</v>
+      </c>
+      <c r="I9" s="12">
+        <v>1</v>
+      </c>
+      <c r="J9" s="12"/>
+      <c r="K9" s="20"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G10" s="5">
+        <v>1</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0.6714</v>
+      </c>
+      <c r="I10" s="5">
+        <v>5.8220000000000001E-2</v>
+      </c>
+      <c r="J10" s="5">
+        <v>3.6768000000000001</v>
+      </c>
+      <c r="K10" s="55">
+        <v>0.04</v>
+      </c>
+      <c r="L10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="7"/>
+      <c r="F11" t="s">
+        <v>121</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <v>0.21609999999999999</v>
+      </c>
+      <c r="I11">
+        <v>1.873E-2</v>
+      </c>
+      <c r="J11">
+        <v>0.39439999999999997</v>
+      </c>
+      <c r="K11" s="8">
+        <v>0.90400000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="7"/>
+      <c r="F12" t="s">
+        <v>122</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0.2263</v>
+      </c>
+      <c r="I12">
+        <v>1.9630000000000002E-2</v>
+      </c>
+      <c r="J12">
+        <v>1.2395</v>
+      </c>
+      <c r="K12" s="8">
+        <v>0.26100000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="7"/>
+      <c r="F13" t="s">
+        <v>123</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <v>0.193</v>
+      </c>
+      <c r="I13">
+        <v>1.6729999999999998E-2</v>
+      </c>
+      <c r="J13">
+        <v>0.35220000000000001</v>
+      </c>
+      <c r="K13" s="8">
+        <v>0.94899999999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="7"/>
+      <c r="F14" t="s">
+        <v>124</v>
+      </c>
+      <c r="G14">
+        <v>56</v>
+      </c>
+      <c r="H14">
+        <v>10.2263</v>
+      </c>
+      <c r="I14">
+        <v>0.88668999999999998</v>
+      </c>
+      <c r="K14" s="8"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="11"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="G15" s="12">
+        <v>64</v>
+      </c>
+      <c r="H15" s="12">
+        <v>11.533099999999999</v>
+      </c>
+      <c r="I15" s="12">
+        <v>1</v>
+      </c>
+      <c r="J15" s="12"/>
+      <c r="K15" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD79A22-9206-4C47-A3DF-875AF2E44DC7}">
   <dimension ref="A1:J87"/>
   <sheetViews>
@@ -3001,14 +3441,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -4783,12 +5223,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{749E9FE6-41D0-6545-9981-B8F3B53996AD}">
   <dimension ref="A1:J83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4801,21 +5241,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="86" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -5540,10 +5980,10 @@
       <c r="H36">
         <v>2</v>
       </c>
-      <c r="I36" s="53" t="s">
+      <c r="I36" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="J36" s="52" t="s">
+      <c r="J36" s="37" t="s">
         <v>33</v>
       </c>
     </row>
@@ -5651,7 +6091,7 @@
       <c r="H41">
         <v>3</v>
       </c>
-      <c r="I41" s="54">
+      <c r="I41" s="49">
         <v>0.27073999999999998</v>
       </c>
     </row>
@@ -5765,7 +6205,7 @@
       <c r="H48">
         <v>2</v>
       </c>
-      <c r="I48" s="55">
+      <c r="I48" s="50">
         <v>1.615E-5</v>
       </c>
       <c r="J48" t="s">
@@ -5787,7 +6227,7 @@
       <c r="H49">
         <v>3</v>
       </c>
-      <c r="I49" s="55">
+      <c r="I49" s="50">
         <v>2.6429999999999999E-12</v>
       </c>
       <c r="J49" t="s">
@@ -5809,7 +6249,7 @@
       <c r="H50">
         <v>1</v>
       </c>
-      <c r="I50" s="56">
+      <c r="I50" s="51">
         <v>2.6239999999999999E-2</v>
       </c>
       <c r="J50" t="s">
@@ -5831,7 +6271,7 @@
       <c r="H51" s="12">
         <v>6</v>
       </c>
-      <c r="I51" s="57">
+      <c r="I51" s="52">
         <v>3.1390000000000002E-7</v>
       </c>
       <c r="J51" t="s">
@@ -5896,7 +6336,7 @@
       <c r="H54">
         <v>1</v>
       </c>
-      <c r="I54" s="56">
+      <c r="I54" s="51">
         <v>6.1919999999999996E-3</v>
       </c>
       <c r="J54" t="s">
@@ -5945,7 +6385,7 @@
       <c r="H56">
         <v>2</v>
       </c>
-      <c r="I56" s="58">
+      <c r="I56" s="53">
         <v>3.7890000000000003E-14</v>
       </c>
       <c r="J56" t="s">
@@ -6112,10 +6552,10 @@
       <c r="H64">
         <v>2</v>
       </c>
-      <c r="I64" s="53" t="s">
+      <c r="I64" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="J64" s="52" t="s">
+      <c r="J64" s="37" t="s">
         <v>33</v>
       </c>
     </row>
@@ -6264,7 +6704,7 @@
       <c r="H71" s="12">
         <v>6</v>
       </c>
-      <c r="I71" s="59">
+      <c r="I71" s="54">
         <v>2.6488000000000001E-2</v>
       </c>
       <c r="J71" t="s">
@@ -6380,10 +6820,10 @@
       <c r="H76">
         <v>2</v>
       </c>
-      <c r="I76" s="53" t="s">
+      <c r="I76" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="J76" s="52" t="s">
+      <c r="J76" s="37" t="s">
         <v>33</v>
       </c>
     </row>
@@ -6466,10 +6906,10 @@
       <c r="H80">
         <v>2</v>
       </c>
-      <c r="I80" s="53" t="s">
+      <c r="I80" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="J80" s="52" t="s">
+      <c r="J80" s="37" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>